<commit_message>
Přidána správa dodavatelů, snad vše ok
</commit_message>
<xml_diff>
--- a/Výkazy/Lukáš Toman.xlsx
+++ b/Výkazy/Lukáš Toman.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Výkaz:</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">Vytvoření scénářu použití </t>
+  </si>
+  <si>
+    <t>Implementace správy dodavatelů</t>
   </si>
 </sst>
 </file>
@@ -425,11 +428,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +460,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>SUM(B7:B1002)</f>
-        <v>11.75</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -525,6 +528,14 @@
       </c>
       <c r="B13" s="8">
         <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>